<commit_message>
Fix time format of month 5
</commit_message>
<xml_diff>
--- a/adhan_excel/helsinki/5.xlsx
+++ b/adhan_excel/helsinki/5.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Päivämäärä
 تاریخ</t>
@@ -43,363 +43,103 @@
     <t>1/5</t>
   </si>
   <si>
-    <t>05:16</t>
-  </si>
-  <si>
-    <t>13:17</t>
-  </si>
-  <si>
-    <t>21:18</t>
-  </si>
-  <si>
-    <t>21:49</t>
-  </si>
-  <si>
     <t>2/5</t>
   </si>
   <si>
-    <t>05:13</t>
-  </si>
-  <si>
-    <t>21:20</t>
-  </si>
-  <si>
-    <t>21:52</t>
-  </si>
-  <si>
     <t>3/5</t>
   </si>
   <si>
-    <t>05:11</t>
-  </si>
-  <si>
-    <t>21:23</t>
-  </si>
-  <si>
-    <t>21:55</t>
-  </si>
-  <si>
     <t>4/5</t>
   </si>
   <si>
-    <t>05:08</t>
-  </si>
-  <si>
-    <t>21:25</t>
-  </si>
-  <si>
-    <t>21:58</t>
-  </si>
-  <si>
     <t>5/5</t>
   </si>
   <si>
-    <t>05:05</t>
-  </si>
-  <si>
-    <t>13:16</t>
-  </si>
-  <si>
-    <t>21:28</t>
-  </si>
-  <si>
-    <t>22:01</t>
-  </si>
-  <si>
     <t>6/5</t>
   </si>
   <si>
-    <t>05:03</t>
-  </si>
-  <si>
-    <t>21:30</t>
-  </si>
-  <si>
-    <t>22:04</t>
-  </si>
-  <si>
     <t>7/5</t>
   </si>
   <si>
-    <t>05:00</t>
-  </si>
-  <si>
-    <t>21:33</t>
-  </si>
-  <si>
-    <t>22:06</t>
-  </si>
-  <si>
     <t>8/5</t>
   </si>
   <si>
-    <t>04:57</t>
-  </si>
-  <si>
-    <t>21:35</t>
-  </si>
-  <si>
-    <t>22:09</t>
-  </si>
-  <si>
     <t>9/5</t>
   </si>
   <si>
-    <t>04:55</t>
-  </si>
-  <si>
-    <t>21:37</t>
-  </si>
-  <si>
-    <t>22:12</t>
-  </si>
-  <si>
     <t>10/5</t>
   </si>
   <si>
-    <t>04:52</t>
-  </si>
-  <si>
-    <t>21:40</t>
-  </si>
-  <si>
-    <t>22:15</t>
-  </si>
-  <si>
     <t>11/5</t>
   </si>
   <si>
-    <t>04:50</t>
-  </si>
-  <si>
-    <t>21:42</t>
-  </si>
-  <si>
-    <t>22:18</t>
-  </si>
-  <si>
     <t>12/5</t>
   </si>
   <si>
-    <t>04:47</t>
-  </si>
-  <si>
-    <t>21:45</t>
-  </si>
-  <si>
-    <t>22:21</t>
-  </si>
-  <si>
     <t>13/5</t>
   </si>
   <si>
-    <t>04:45</t>
-  </si>
-  <si>
-    <t>21:47</t>
-  </si>
-  <si>
-    <t>22:24</t>
-  </si>
-  <si>
     <t>14/5</t>
   </si>
   <si>
-    <t>04:43</t>
-  </si>
-  <si>
-    <t>21:50</t>
-  </si>
-  <si>
-    <t>22:26</t>
-  </si>
-  <si>
     <t>15/5</t>
   </si>
   <si>
-    <t>04:40</t>
-  </si>
-  <si>
-    <t>22:29</t>
-  </si>
-  <si>
     <t>16/5</t>
   </si>
   <si>
-    <t>04:38</t>
-  </si>
-  <si>
-    <t>21:54</t>
-  </si>
-  <si>
-    <t>22:32</t>
-  </si>
-  <si>
     <t>17/5</t>
   </si>
   <si>
-    <t>04:36</t>
-  </si>
-  <si>
-    <t>21:57</t>
-  </si>
-  <si>
-    <t>22:35</t>
-  </si>
-  <si>
     <t>18/5</t>
   </si>
   <si>
-    <t>04:33</t>
-  </si>
-  <si>
-    <t>21:59</t>
-  </si>
-  <si>
-    <t>22:38</t>
-  </si>
-  <si>
     <t>19/5</t>
   </si>
   <si>
-    <t>04:31</t>
-  </si>
-  <si>
-    <t>22:40</t>
-  </si>
-  <si>
     <t>20/5</t>
   </si>
   <si>
-    <t>04:29</t>
-  </si>
-  <si>
-    <t>22:43</t>
-  </si>
-  <si>
     <t>21/5</t>
   </si>
   <si>
-    <t>04:27</t>
-  </si>
-  <si>
-    <t>22:46</t>
-  </si>
-  <si>
     <t>22/5</t>
   </si>
   <si>
-    <t>04:25</t>
-  </si>
-  <si>
-    <t>22:08</t>
-  </si>
-  <si>
-    <t>22:49</t>
-  </si>
-  <si>
     <t>23/5</t>
   </si>
   <si>
-    <t>04:23</t>
-  </si>
-  <si>
-    <t>22:10</t>
-  </si>
-  <si>
-    <t>22:51</t>
-  </si>
-  <si>
     <t>24/5</t>
   </si>
   <si>
-    <t>04:21</t>
-  </si>
-  <si>
-    <t>22:54</t>
-  </si>
-  <si>
     <t>25/5</t>
   </si>
   <si>
-    <t>04:19</t>
-  </si>
-  <si>
-    <t>22:57</t>
-  </si>
-  <si>
     <t>26/5</t>
   </si>
   <si>
-    <t>04:17</t>
-  </si>
-  <si>
-    <t>22:17</t>
-  </si>
-  <si>
-    <t>22:59</t>
-  </si>
-  <si>
     <t>27/5</t>
   </si>
   <si>
-    <t>04:15</t>
-  </si>
-  <si>
-    <t>22:19</t>
-  </si>
-  <si>
-    <t>23:02</t>
-  </si>
-  <si>
     <t>28/5</t>
   </si>
   <si>
-    <t>04:13</t>
-  </si>
-  <si>
-    <t>23:05</t>
-  </si>
-  <si>
     <t>29/5</t>
   </si>
   <si>
-    <t>04:12</t>
-  </si>
-  <si>
-    <t>22:23</t>
-  </si>
-  <si>
-    <t>23:07</t>
-  </si>
-  <si>
     <t>30/5</t>
   </si>
   <si>
-    <t>04:10</t>
-  </si>
-  <si>
-    <t>22:25</t>
-  </si>
-  <si>
-    <t>23:10</t>
-  </si>
-  <si>
     <t>31/5</t>
-  </si>
-  <si>
-    <t>04:08</t>
-  </si>
-  <si>
-    <t>23:12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="h&quot;:&quot;mm"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -447,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -460,8 +200,11 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -715,17 +458,17 @@
       <c r="B2" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
+      <c r="C2" s="3">
+        <v>0.21944444444444444</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.8875</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.9090277777777778</v>
       </c>
       <c r="G2" s="3">
         <v>0.0</v>
@@ -733,22 +476,22 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
+      <c r="C3" s="5">
+        <v>0.21736111111111112</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.9111111111111111</v>
       </c>
       <c r="G3" s="3">
         <v>0.0</v>
@@ -756,22 +499,22 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
+      <c r="C4" s="4">
+        <v>0.21597222222222223</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.8909722222222223</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.9131944444444444</v>
       </c>
       <c r="G4" s="3">
         <v>0.0</v>
@@ -779,22 +522,22 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>23</v>
+      <c r="C5" s="4">
+        <v>0.21388888888888888</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.8923611111111112</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.9152777777777777</v>
       </c>
       <c r="G5" s="3">
         <v>0.0</v>
@@ -802,22 +545,22 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>28</v>
+      <c r="C6" s="4">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.8944444444444445</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.9173611111111111</v>
       </c>
       <c r="G6" s="3">
         <v>0.0</v>
@@ -825,22 +568,22 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>32</v>
+      <c r="C7" s="4">
+        <v>0.21041666666666667</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.9194444444444444</v>
       </c>
       <c r="G7" s="3">
         <v>0.0</v>
@@ -848,22 +591,22 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>36</v>
+      <c r="C8" s="4">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.8979166666666667</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.9208333333333333</v>
       </c>
       <c r="G8" s="3">
         <v>0.0</v>
@@ -871,22 +614,22 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>40</v>
+      <c r="C9" s="4">
+        <v>0.20625</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.8993055555555556</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.9229166666666667</v>
       </c>
       <c r="G9" s="3">
         <v>0.0</v>
@@ -894,22 +637,22 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>44</v>
+      <c r="C10" s="4">
+        <v>0.2048611111111111</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.9006944444444445</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.925</v>
       </c>
       <c r="G10" s="3">
         <v>0.0</v>
@@ -917,22 +660,22 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>48</v>
+      <c r="C11" s="4">
+        <v>0.20277777777777778</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.9027777777777778</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.9270833333333334</v>
       </c>
       <c r="G11" s="3">
         <v>0.0</v>
@@ -940,22 +683,22 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B12" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>52</v>
+      <c r="C12" s="4">
+        <v>0.2013888888888889</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.9041666666666667</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.9291666666666667</v>
       </c>
       <c r="G12" s="3">
         <v>0.0</v>
@@ -963,459 +706,459 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="4">
+        <v>0.19930555555555557</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.90625</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.93125</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.9076388888888889</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.19652777777777777</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.9097222222222222</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.9347222222222222</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.9111111111111111</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.9368055555555556</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.19305555555555556</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.9125</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.9388888888888889</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.19166666666666668</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.9145833333333333</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.9409722222222222</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.9159722222222222</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.9430555555555555</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.18819444444444444</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.9173611111111111</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="B21" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.18680555555555556</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.9194444444444444</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.9465277777777777</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.18541666666666667</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.9208333333333333</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.9486111111111111</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="B23" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.1840277777777778</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.9222222222222223</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.9506944444444444</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.18263888888888888</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.9236111111111112</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.9520833333333333</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.18125</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.925</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.9541666666666667</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.1798611111111111</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.9270833333333334</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.95625</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="B27" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.17847222222222223</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.9284722222222223</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.9576388888888889</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.17708333333333334</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.9298611111111111</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0.9597222222222223</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.17569444444444443</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.93125</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0.9618055555555556</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.07361111111111111</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.175</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.9326388888888889</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0.9631944444444445</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B28" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G28" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="3">
-        <v>0.07361111111111111</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>118</v>
-      </c>
       <c r="B31" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>121</v>
+      <c r="C31" s="4">
+        <v>0.1736111111111111</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.9340277777777778</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0.9652777777777778</v>
       </c>
       <c r="G31" s="3">
         <v>0.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>122</v>
+      <c r="A32" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B32" s="3">
         <v>0.07361111111111111</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>124</v>
+      <c r="C32" s="4">
+        <v>0.17222222222222222</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.9347222222222222</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0.9666666666666667</v>
       </c>
       <c r="G32" s="3">
         <v>0.0</v>

</xml_diff>